<commit_message>
rule of half and corrected sign of PT emissions change
</commit_message>
<xml_diff>
--- a/CBA.xlsx
+++ b/CBA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanelmaheinonen/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a630b34756993743/Desktop/ETHZ/Transport Planning Methods/TransportPlanning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7917CEA6-7AB6-7840-849C-A049323EA15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{7917CEA6-7AB6-7840-849C-A049323EA15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC0CC021-1988-4AB7-9551-7490297425D0}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="500" windowWidth="29220" windowHeight="14380" xr2:uid="{CB19214C-161C-4FCD-BB74-FBBD26C9B7EC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CB19214C-161C-4FCD-BB74-FBBD26C9B7EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Project 2" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -72,39 +69,6 @@
             <family val="2"/>
           </rPr>
           <t>Calculated from official swiss population scenario estimates 2020 and 2050, assuming a constant growth rate</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J36" authorId="0" shapeId="0" xr:uid="{158D98E5-FEA1-3348-BFE4-5E0C43B26646}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Heinonen  Sanelma:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Assuming car travel time does not change (these benefits will be accounted for by congestion benefits)</t>
         </r>
       </text>
     </comment>
@@ -227,39 +191,6 @@
     <author>Heinonen  Sanelma</author>
   </authors>
   <commentList>
-    <comment ref="I21" authorId="0" shapeId="0" xr:uid="{454664A0-F363-B04E-8EAE-396817BBEC05}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Heinonen  Sanelma:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Assuming car travel time does not change (these benefits will be accounted for by congestion benefits)</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="L21" authorId="0" shapeId="0" xr:uid="{FFC213B8-785A-9245-B331-3D07429FD761}">
       <text>
         <r>
@@ -374,7 +305,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="97">
   <si>
     <t>Weekly benefits</t>
   </si>
@@ -608,12 +539,6 @@
   </si>
   <si>
     <t>Aggregate travel times savings (CHF)</t>
-  </si>
-  <si>
-    <t>Aggregate original travel time (hrs)</t>
-  </si>
-  <si>
-    <t>New aggregate travel time (hrs)</t>
   </si>
   <si>
     <t>Congestion cost (CHF) per pkm</t>
@@ -704,9 +629,6 @@
     <t>Would be good to get a lower travel time here to account for less congestions?</t>
   </si>
   <si>
-    <t>How to account for rule of 1/2 that is in the slides? Less benefits from induced demand</t>
-  </si>
-  <si>
     <t>Should try to find an estimate for how TT will change with less congestion?</t>
   </si>
   <si>
@@ -720,18 +642,25 @@
   </si>
   <si>
     <t>Annual benefits</t>
+  </si>
+  <si>
+    <t>Existing demand travel time savings (CHF)</t>
+  </si>
+  <si>
+    <t>Induced demand travel time savings (CHF)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$CHF-100C]_-;\-* #,##0.00\ [$CHF-100C]_-;_-* &quot;-&quot;??\ [$CHF-100C]_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="174" formatCode="_-* #,##0\ [$CHF-100C]_-;\-* #,##0\ [$CHF-100C]_-;_-* &quot;-&quot;??\ [$CHF-100C]_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0\ [$CHF-100C]_-;\-* #,##0\ [$CHF-100C]_-;_-* &quot;-&quot;??\ [$CHF-100C]_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="170" formatCode="0.0%"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -914,22 +843,17 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -945,8 +869,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -955,22 +879,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -986,15 +908,16 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="174" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1313,55 +1236,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D083A40F-175A-4EEC-B4D7-09BE1D9F546C}">
   <dimension ref="A1:R116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q36" sqref="Q36"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="55" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="47.5" customWidth="1"/>
-    <col min="5" max="5" width="5.5" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
-    <col min="7" max="7" width="29.83203125" customWidth="1"/>
-    <col min="8" max="8" width="17.5" customWidth="1"/>
-    <col min="9" max="9" width="12.5" customWidth="1"/>
-    <col min="10" max="11" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="19.6328125" customWidth="1"/>
+    <col min="4" max="4" width="47.453125" customWidth="1"/>
+    <col min="5" max="5" width="5.453125" customWidth="1"/>
+    <col min="6" max="6" width="18.36328125" customWidth="1"/>
+    <col min="7" max="7" width="29.81640625" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" customWidth="1"/>
+    <col min="10" max="11" width="17.453125" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="15" max="15" width="11.83203125" customWidth="1"/>
-    <col min="16" max="16" width="12.83203125" customWidth="1"/>
-    <col min="17" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="12.1640625" customWidth="1"/>
+    <col min="15" max="15" width="11.81640625" customWidth="1"/>
+    <col min="16" max="16" width="12.81640625" customWidth="1"/>
+    <col min="17" max="17" width="11.36328125" customWidth="1"/>
+    <col min="18" max="18" width="12.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="C3" s="6" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="7">
         <v>8000</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C4" s="1"/>
       <c r="G4" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
@@ -1378,14 +1301,14 @@
       <c r="G5" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="7">
         <v>2</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1396,11 +1319,11 @@
       <c r="G6" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="7">
         <v>65000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
@@ -1411,11 +1334,11 @@
       <c r="G7" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="7">
         <v>320000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
@@ -1426,11 +1349,11 @@
       <c r="G8" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1441,68 +1364,68 @@
       <c r="G9" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="7">
         <v>2200</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="C10" s="12" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="10">
         <f>(D3*H12*H5)/2</f>
         <v>640000000</v>
       </c>
       <c r="G10" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="7">
         <v>470</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="C11" s="5" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="5">
         <f>SUM(D5:D10)</f>
         <v>1728200000</v>
       </c>
       <c r="G11" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="7">
         <v>4200000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G12" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="7">
         <v>80000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C13" s="5"/>
-      <c r="D13" s="7"/>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C13" s="4"/>
+      <c r="D13" s="5"/>
       <c r="G13" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="24">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C14" s="5"/>
-      <c r="D14" s="7"/>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="B15" s="14" t="s">
+    <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B15" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1512,69 +1435,68 @@
         <f>D7*((1+H13)^(-15)+(1+H13)^(-30)+(1+H13)^-(45))</f>
         <v>52672669.125554681</v>
       </c>
-      <c r="F15" s="4"/>
       <c r="G15" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="7">
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="C16" s="12" t="s">
+    <row r="16" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="C16" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="10">
         <f>D8*((1+H13)^-10 + (1+H13)^-20 +(1+ H13)^-30 + (1+H13)^-40 + (1+H13)^-50 )</f>
         <v>19037518.158102311</v>
       </c>
       <c r="G16" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="7">
         <v>0.05</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="C17" s="5" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C17" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="5">
         <f>D15+D16</f>
         <v>71710187.283656985</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C18" s="5"/>
-      <c r="D18" s="7"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
       <c r="G18" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B19" s="5" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B19" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="8">
+      <c r="C19" s="4"/>
+      <c r="D19" s="2">
         <f>H16*(D11+D17)</f>
         <v>89995509.36418286</v>
       </c>
       <c r="G19" t="s">
         <v>56</v>
       </c>
-      <c r="H19" s="10">
+      <c r="H19" s="7">
         <v>15</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="5"/>
+      <c r="C20" s="4"/>
       <c r="D20" s="2">
         <f>(D17+D11)*H15</f>
         <v>138593084.4208416</v>
@@ -1582,70 +1504,70 @@
       <c r="G20" t="s">
         <v>57</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H20" s="7">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="5"/>
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C21" s="4"/>
       <c r="D21" s="2"/>
       <c r="G21" t="s">
         <v>58</v>
       </c>
-      <c r="H21" s="10">
+      <c r="H21" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="37">
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="29"/>
+      <c r="D22" s="32">
         <f>D11+D17+D19+D20</f>
         <v>2028498781.0686817</v>
       </c>
-      <c r="F22" s="9"/>
+      <c r="F22" s="6"/>
       <c r="G22" t="s">
         <v>59</v>
       </c>
-      <c r="H22" s="10">
+      <c r="H22" s="7">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C23" s="1"/>
-      <c r="D23" s="7"/>
-      <c r="F23" s="9"/>
+      <c r="D23" s="5"/>
+      <c r="F23" s="6"/>
       <c r="G23" t="s">
         <v>61</v>
       </c>
-      <c r="H23" s="10">
+      <c r="H23" s="7">
         <v>18</v>
       </c>
-      <c r="I23" s="38" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I23" s="33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C24" s="1"/>
-      <c r="D24" s="7"/>
-      <c r="F24" s="9"/>
+      <c r="D24" s="5"/>
+      <c r="F24" s="6"/>
       <c r="G24" t="s">
         <v>62</v>
       </c>
-      <c r="H24" s="10">
+      <c r="H24" s="7">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="C25" s="40" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C25" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="D25" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F25" s="9"/>
+      <c r="F25" s="6"/>
       <c r="G25" t="s">
         <v>66</v>
       </c>
@@ -1654,170 +1576,168 @@
         <v>19.8</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="16">
+      <c r="C26" s="13">
         <v>452</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D26" s="13">
         <v>412</v>
       </c>
-      <c r="F26" s="9"/>
+      <c r="F26" s="6"/>
       <c r="G26" t="s">
         <v>63</v>
       </c>
-      <c r="H26" s="10">
+      <c r="H26" s="7">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="16">
+      <c r="C27" s="13">
         <v>322</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D27" s="13">
         <v>444</v>
       </c>
-      <c r="F27" s="9"/>
+      <c r="F27" s="6"/>
       <c r="G27" t="s">
         <v>64</v>
       </c>
-      <c r="H27" s="10">
+      <c r="H27" s="7">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
-      <c r="B28" s="39" t="s">
+      <c r="B28" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="16">
+      <c r="C28" s="13">
         <v>27</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="13">
         <v>35</v>
       </c>
-      <c r="F28" s="9"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="11"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F28" s="6"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="8"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="16">
+      <c r="C29" s="13">
         <v>6</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="13">
         <v>8</v>
       </c>
-      <c r="F29" s="9"/>
+      <c r="F29" s="6"/>
       <c r="G29" t="s">
-        <v>80</v>
-      </c>
-      <c r="H29" s="28">
+        <v>78</v>
+      </c>
+      <c r="H29" s="24">
         <v>6.1500000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
-      <c r="B30" s="39" t="s">
+      <c r="B30" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="1">
         <f>SUM(C26:C29)</f>
         <v>807</v>
       </c>
-      <c r="D30" s="18">
+      <c r="D30" s="15">
         <f>SUM(D26:D29)</f>
         <v>899</v>
       </c>
-      <c r="F30" s="9"/>
-    </row>
-    <row r="31" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
         <v>65</v>
       </c>
       <c r="B31" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="19">
+      <c r="C31" s="16">
         <f>C30*52</f>
         <v>41964</v>
       </c>
-      <c r="D31" s="19">
+      <c r="D31" s="16">
         <f>D30*52</f>
         <v>46748</v>
       </c>
-      <c r="F31" s="9"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C32" s="1"/>
-      <c r="D32" s="7"/>
-      <c r="F32" s="9"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D32" s="5"/>
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C33" s="1"/>
-      <c r="D33" s="7"/>
-      <c r="F33" s="9"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D33" s="5"/>
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C34" s="1"/>
-      <c r="D34" s="24"/>
-      <c r="F34" s="9"/>
+      <c r="D34" s="3"/>
+      <c r="F34" s="6"/>
       <c r="H34" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="K34" s="38" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+      <c r="K34" s="33"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C35" s="1"/>
-      <c r="D35" s="7"/>
-      <c r="F35" s="9"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25" t="s">
+      <c r="D35" s="5"/>
+      <c r="F35" s="6"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="20"/>
-      <c r="M35" s="20" t="s">
+      <c r="J35" s="21"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="N35" s="20"/>
-      <c r="O35" s="20"/>
-      <c r="P35" s="20"/>
-      <c r="Q35" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="R35" s="26"/>
-    </row>
-    <row r="36" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+      <c r="N35" s="17"/>
+      <c r="O35" s="17"/>
+      <c r="P35" s="17"/>
+      <c r="Q35" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="R35" s="22"/>
+    </row>
+    <row r="36" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C36" s="1"/>
       <c r="G36" t="s">
         <v>13</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="H36" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K36" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="K36" s="4" t="s">
         <v>73</v>
       </c>
       <c r="L36" s="1" t="s">
@@ -1832,17 +1752,17 @@
       <c r="O36" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="P36" s="5" t="s">
+      <c r="P36" s="4" t="s">
         <v>10</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>1</v>
       </c>
@@ -1854,45 +1774,43 @@
       </c>
       <c r="D37" s="2">
         <f>SUM(K37:K38)</f>
-        <v>719.95199999999977</v>
+        <v>1213.3439999999998</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H37" s="10">
+      <c r="H37" s="7">
         <v>23.3</v>
       </c>
       <c r="I37">
-        <f>(C26*H23)/60</f>
-        <v>135.6</v>
+        <v>0</v>
       </c>
       <c r="J37" s="1">
-        <f>D26*H23/60</f>
-        <v>123.6</v>
-      </c>
-      <c r="K37" s="5">
-        <f>(I37-J37)*H37</f>
-        <v>279.60000000000002</v>
+        <v>0</v>
+      </c>
+      <c r="K37" s="4">
+        <f>I37+J37</f>
+        <v>0</v>
       </c>
       <c r="L37">
         <f>C26*H19-D26*H19</f>
         <v>600</v>
       </c>
-      <c r="M37" s="10">
+      <c r="M37" s="7">
         <v>192</v>
       </c>
       <c r="N37">
         <f>M37/1000000</f>
         <v>1.92E-4</v>
       </c>
-      <c r="O37" s="10">
+      <c r="O37" s="7">
         <v>90</v>
       </c>
       <c r="P37" s="3">
         <f>L37*N37*O37</f>
         <v>10.368</v>
       </c>
-      <c r="Q37" s="10">
+      <c r="Q37" s="7">
         <f>(0.012+0.031)/2</f>
         <v>2.1499999999999998E-2</v>
       </c>
@@ -1901,7 +1819,7 @@
         <v>12.899999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="C38" s="1" t="s">
         <v>9</v>
       </c>
@@ -1912,33 +1830,33 @@
       <c r="G38" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H38" s="10">
+      <c r="H38" s="7">
         <v>14.4</v>
       </c>
       <c r="I38">
-        <f>(C27*H24)/60</f>
-        <v>177.1</v>
+        <f>(C27*(H24-H25)*H38)/60</f>
+        <v>1020.0959999999999</v>
       </c>
       <c r="J38" s="1">
-        <f>D27*H25/60</f>
-        <v>146.52000000000001</v>
-      </c>
-      <c r="K38" s="5">
-        <f>(I38-J38)*H38</f>
-        <v>440.3519999999998</v>
+        <f>0.5*(D27-C27)*(H24-H25)*H38/60</f>
+        <v>193.24799999999999</v>
+      </c>
+      <c r="K38" s="4">
+        <f>I38+J38</f>
+        <v>1213.3439999999998</v>
       </c>
       <c r="L38">
         <f>D27*H20-C27*H20</f>
         <v>1708</v>
       </c>
-      <c r="M38" s="10">
+      <c r="M38" s="7">
         <v>35</v>
       </c>
       <c r="N38">
         <f t="shared" ref="N38:N40" si="0">M38/1000000</f>
         <v>3.4999999999999997E-5</v>
       </c>
-      <c r="O38" s="10">
+      <c r="O38" s="7">
         <v>90</v>
       </c>
       <c r="P38" s="3">
@@ -1948,9 +1866,9 @@
       <c r="Q38">
         <v>0</v>
       </c>
-      <c r="R38" s="22"/>
-    </row>
-    <row r="39" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="R38" s="19"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C39" t="s">
         <v>67</v>
       </c>
@@ -1961,22 +1879,22 @@
       <c r="G39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H39" s="21"/>
-      <c r="I39" s="22"/>
-      <c r="J39" s="23"/>
-      <c r="K39" s="23"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
       <c r="L39">
         <f>D28*H21-C28*H21</f>
         <v>24</v>
       </c>
-      <c r="M39" s="10">
+      <c r="M39" s="7">
         <v>0</v>
       </c>
       <c r="N39">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O39" s="10">
+      <c r="O39" s="7">
         <v>90</v>
       </c>
       <c r="P39" s="3">
@@ -1986,28 +1904,28 @@
       <c r="Q39">
         <v>0</v>
       </c>
-      <c r="R39" s="22"/>
-    </row>
-    <row r="40" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="R39" s="19"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="G40" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H40" s="21"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="22"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
       <c r="L40">
         <f>D29*H22-C29*H22</f>
         <v>16</v>
       </c>
-      <c r="M40" s="10">
+      <c r="M40" s="7">
         <v>0</v>
       </c>
       <c r="N40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O40" s="10">
+      <c r="O40" s="7">
         <v>90</v>
       </c>
       <c r="P40" s="3">
@@ -2017,688 +1935,688 @@
       <c r="Q40">
         <v>0</v>
       </c>
-      <c r="R40" s="22"/>
-    </row>
-    <row r="41" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="C41" s="5" t="s">
+      <c r="R40" s="19"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="C41" s="4" t="s">
         <v>53</v>
       </c>
       <c r="D41" s="2">
         <f>SUM(D37:D39)</f>
-        <v>748.60019999999975</v>
-      </c>
-      <c r="F41" s="9"/>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+        <v>1241.9921999999999</v>
+      </c>
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B43" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D43" s="2">
         <f>52*D41</f>
-        <v>38927.210399999989</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>64583.594399999994</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="32" t="s">
+    <row r="45" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B45" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="30"/>
+      <c r="D45" s="31">
+        <f>SUM(B56:B116)</f>
+        <v>2379946.5361761739</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A48" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48" s="42">
+        <f>D45/D22</f>
+        <v>1.1732550980002748E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>81</v>
       </c>
-      <c r="C45" s="35"/>
-      <c r="D45" s="36">
-        <f>SUM(B56:B116)</f>
-        <v>1434492.4653881008</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="B48" s="47">
-        <f>D45/D22</f>
-        <v>7.0716949833825467E-4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>83</v>
-      </c>
-      <c r="B53" s="27">
+      <c r="B53" s="23">
         <f>H29</f>
         <v>6.1500000000000001E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>84</v>
-      </c>
-      <c r="B54" s="29">
+        <v>82</v>
+      </c>
+      <c r="B54" s="45">
         <f>H13</f>
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>85</v>
-      </c>
-      <c r="B55" s="29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="B55" s="25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>0</v>
       </c>
-      <c r="B56" s="31">
-        <f>$D$43*(1+$B$54)^-A56*(1+$B$53)^A56</f>
-        <v>38927.210399999989</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B56" s="26">
+        <f t="shared" ref="B56:B87" si="1">$D$43*(1+$B$54)^-A56*(1+$B$53)^A56</f>
+        <v>64583.594399999994</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>1</v>
       </c>
-      <c r="B57" s="31">
-        <f>$D$43*(1+$B$54)^-A57*(1+$B$53)^A57</f>
-        <v>38211.329506302442</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B57" s="26">
+        <f t="shared" si="1"/>
+        <v>63395.886346887812</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>2</v>
       </c>
-      <c r="B58" s="31">
-        <f>$D$43*(1+$B$54)^-A58*(1+$B$53)^A58</f>
-        <v>37508.61383684507</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B58" s="26">
+        <f t="shared" si="1"/>
+        <v>62230.020534557239</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59">
         <f>A58+1</f>
         <v>3</v>
       </c>
-      <c r="B59" s="31">
-        <f>$D$43*(1+$B$54)^-A59*(1+$B$53)^A59</f>
-        <v>36818.821279943091</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B59" s="26">
+        <f t="shared" si="1"/>
+        <v>61085.595278872948</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60">
-        <f t="shared" ref="A60:A116" si="1">A59+1</f>
+        <f t="shared" ref="A60:A116" si="2">A59+1</f>
         <v>4</v>
       </c>
-      <c r="B60" s="31">
-        <f>$D$43*(1+$B$54)^-A60*(1+$B$53)^A60</f>
-        <v>36141.714176404632</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B60" s="26">
+        <f t="shared" si="1"/>
+        <v>59962.216282768815</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="B61" s="26">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="B61" s="31">
-        <f>$D$43*(1+$B$54)^-A61*(1+$B$53)^A61</f>
-        <v>35477.059237648311</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+        <v>58859.496500397894</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B62" s="26">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="B62" s="31">
-        <f>$D$43*(1+$B$54)^-A62*(1+$B$53)^A62</f>
-        <v>34824.627465326696</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+        <v>57777.056003780832</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="B63" s="26">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="B63" s="31">
-        <f>$D$43*(1+$B$54)^-A63*(1+$B$53)^A63</f>
-        <v>34184.194072427759</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+        <v>56714.521851906429</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B64" s="26">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="B64" s="31">
-        <f>$D$43*(1+$B$54)^-A64*(1+$B$53)^A64</f>
-        <v>33555.538405827509</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+        <v>55671.52796223967</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="B65" s="26">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="B65" s="31">
-        <f>$D$43*(1+$B$54)^-A65*(1+$B$53)^A65</f>
-        <v>32938.443870266696</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+        <v>54647.71498459264</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="B66" s="26">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="B66" s="31">
-        <f>$D$43*(1+$B$54)^-A66*(1+$B$53)^A66</f>
-        <v>32332.697853725695</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+        <v>53642.730177315025</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="B67" s="26">
         <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="B67" s="31">
-        <f>$D$43*(1+$B$54)^-A67*(1+$B$53)^A67</f>
-        <v>31738.091654171807</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+        <v>52656.227285761466</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="B68" s="26">
         <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="B68" s="31">
-        <f>$D$43*(1+$B$54)^-A68*(1+$B$53)^A68</f>
-        <v>31154.420407653637</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+        <v>51687.86642299407</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="B69" s="26">
         <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="B69" s="31">
-        <f>$D$43*(1+$B$54)^-A69*(1+$B$53)^A69</f>
-        <v>30581.483017717757</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+        <v>50737.313952678516</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="B70" s="26">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="B70" s="31">
-        <f>$D$43*(1+$B$54)^-A70*(1+$B$53)^A70</f>
-        <v>30019.082086123643</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+        <v>49804.242374134148</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="B71" s="26">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="B71" s="31">
-        <f>$D$43*(1+$B$54)^-A71*(1+$B$53)^A71</f>
-        <v>29467.023844832485</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+        <v>48888.330209497624</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72">
         <f>A71+1</f>
         <v>16</v>
       </c>
-      <c r="B72" s="31">
-        <f>$D$43*(1+$B$54)^-A72*(1+$B$53)^A72</f>
-        <v>28925.118089247037</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B72" s="26">
+        <f t="shared" si="1"/>
+        <v>47989.261892962</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="B73" s="26">
         <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="B73" s="31">
-        <f>$D$43*(1+$B$54)^-A73*(1+$B$53)^A73</f>
-        <v>28393.178112678939</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+        <v>47106.727662052414</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="B74" s="26">
         <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="B74" s="31">
-        <f>$D$43*(1+$B$54)^-A74*(1+$B$53)^A74</f>
-        <v>27871.020642021376</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+        <v>46240.423450901493</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="B75" s="26">
         <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="B75" s="31">
-        <f>$D$43*(1+$B$54)^-A75*(1+$B$53)^A75</f>
-        <v>27358.465774604694</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+        <v>45390.050785487358</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B76" s="26">
         <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="B76" s="31">
-        <f>$D$43*(1+$B$54)^-A76*(1+$B$53)^A76</f>
-        <v>26855.336916213186</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+        <v>44555.316680798162</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="B77" s="26">
         <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="B77" s="31">
-        <f>$D$43*(1+$B$54)^-A77*(1+$B$53)^A77</f>
-        <v>26361.460720241856</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+        <v>43735.933539887883</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="B78" s="26">
         <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="B78" s="31">
-        <f>$D$43*(1+$B$54)^-A78*(1+$B$53)^A78</f>
-        <v>25876.667027972046</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+        <v>42931.619054788491</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="B79" s="26">
         <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="B79" s="31">
-        <f>$D$43*(1+$B$54)^-A79*(1+$B$53)^A79</f>
-        <v>25400.788809945443</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+        <v>42142.096109244332</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="B80" s="26">
         <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="B80" s="31">
-        <f>$D$43*(1+$B$54)^-A80*(1+$B$53)^A80</f>
-        <v>24933.662108416207</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+        <v>41367.092683235314</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="B81" s="26">
         <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="B81" s="31">
-        <f>$D$43*(1+$B$54)^-A81*(1+$B$53)^A81</f>
-        <v>24475.12598086143</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+        <v>40606.341759255811</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="B82" s="26">
         <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="B82" s="31">
-        <f>$D$43*(1+$B$54)^-A82*(1+$B$53)^A82</f>
-        <v>24025.022444530478</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+        <v>39859.581230317322</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="B83" s="26">
         <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="B83" s="31">
-        <f>$D$43*(1+$B$54)^-A83*(1+$B$53)^A83</f>
-        <v>23583.196422013985</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+        <v>39126.553809642697</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="B84" s="26">
         <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="B84" s="31">
-        <f>$D$43*(1+$B$54)^-A84*(1+$B$53)^A84</f>
-        <v>23149.495687814029</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+        <v>38407.006942021479</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85">
         <f>A84+1</f>
         <v>29</v>
       </c>
-      <c r="B85" s="31">
-        <f>$D$43*(1+$B$54)^-A85*(1+$B$53)^A85</f>
-        <v>22723.77081589666</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B85" s="26">
+        <f t="shared" si="1"/>
+        <v>37700.69271679502</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="B86" s="26">
         <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="B86" s="31">
-        <f>$D$43*(1+$B$54)^-A86*(1+$B$53)^A86</f>
-        <v>22305.875128209209</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37007.36778244227</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="B87" s="26">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="B87" s="31">
-        <f>$D$43*(1+$B$54)^-A87*(1+$B$53)^A87</f>
-        <v>21895.664644144086</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+        <v>36326.793262735882</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="B88" s="31">
-        <f>$D$43*(1+$B$54)^-A88*(1+$B$53)^A88</f>
-        <v>21492.998030932271</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B88" s="26">
+        <f t="shared" ref="B88:B119" si="3">$D$43*(1+$B$54)^-A88*(1+$B$53)^A88</f>
+        <v>35658.734674440704</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="B89" s="31">
-        <f>$D$43*(1+$B$54)^-A89*(1+$B$53)^A89</f>
-        <v>21097.736554948791</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B89" s="26">
+        <f t="shared" si="3"/>
+        <v>35002.961846525388</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="B90" s="31">
-        <f>$D$43*(1+$B$54)^-A90*(1+$B$53)^A90</f>
-        <v>20709.744033913881</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B90" s="26">
+        <f t="shared" si="3"/>
+        <v>34359.248840860026</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="B91" s="31">
-        <f>$D$43*(1+$B$54)^-A91*(1+$B$53)^A91</f>
-        <v>20328.886789973127</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B91" s="26">
+        <f t="shared" si="3"/>
+        <v>33727.37387437201</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="B92" s="31">
-        <f>$D$43*(1+$B$54)^-A92*(1+$B$53)^A92</f>
-        <v>19955.033603640451</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B92" s="26">
+        <f t="shared" si="3"/>
+        <v>33107.119242633569</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="B93" s="31">
-        <f>$D$43*(1+$B$54)^-A93*(1+$B$53)^A93</f>
-        <v>19588.055668588138</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B93" s="26">
+        <f t="shared" si="3"/>
+        <v>32498.271244854408</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="B94" s="31">
-        <f>$D$43*(1+$B$54)^-A94*(1+$B$53)^A94</f>
-        <v>19227.826547268258</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B94" s="26">
+        <f t="shared" si="3"/>
+        <v>31900.620110253927</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="B95" s="31">
-        <f>$D$43*(1+$B$54)^-A95*(1+$B$53)^A95</f>
-        <v>18874.222127350196</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B95" s="26">
+        <f t="shared" si="3"/>
+        <v>31313.959925787301</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="B96" s="31">
-        <f>$D$43*(1+$B$54)^-A96*(1+$B$53)^A96</f>
-        <v>18527.120578959424</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B96" s="26">
+        <f t="shared" si="3"/>
+        <v>30738.08856520088</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="B97" s="31">
-        <f>$D$43*(1+$B$54)^-A97*(1+$B$53)^A97</f>
-        <v>18186.402312702467</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B97" s="26">
+        <f t="shared" si="3"/>
+        <v>30172.807619392064</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98">
         <f>A97+1</f>
         <v>42</v>
       </c>
-      <c r="B98" s="31">
-        <f>$D$43*(1+$B$54)^-A98*(1+$B$53)^A98</f>
-        <v>17851.949938463986</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B98" s="26">
+        <f t="shared" si="3"/>
+        <v>29617.922328050081</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="B99" s="31">
-        <f>$D$43*(1+$B$54)^-A99*(1+$B$53)^A99</f>
-        <v>17523.6482249615</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B99" s="26">
+        <f t="shared" si="3"/>
+        <v>29073.241512553737</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="B100" s="31">
-        <f>$D$43*(1+$B$54)^-A100*(1+$B$53)^A100</f>
-        <v>17201.384060043925</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B100" s="26">
+        <f t="shared" si="3"/>
+        <v>28538.57751010338</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101">
         <f>A100+1</f>
         <v>45</v>
       </c>
-      <c r="B101" s="31">
-        <f>$D$43*(1+$B$54)^-A101*(1+$B$53)^A101</f>
-        <v>16885.046411720188</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B101" s="26">
+        <f t="shared" si="3"/>
+        <v>28013.746109063908</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="B102" s="31">
-        <f>$D$43*(1+$B$54)^-A102*(1+$B$53)^A102</f>
-        <v>16574.526289904654</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B102" s="26">
+        <f t="shared" si="3"/>
+        <v>27498.566485497231</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="B103" s="31">
-        <f>$D$43*(1+$B$54)^-A103*(1+$B$53)^A103</f>
-        <v>16269.716708865921</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B103" s="26">
+        <f t="shared" si="3"/>
+        <v>26992.8611408615</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="B104" s="31">
-        <f>$D$43*(1+$B$54)^-A104*(1+$B$53)^A104</f>
-        <v>15970.51265036629</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B104" s="26">
+        <f t="shared" si="3"/>
+        <v>26496.455840856393</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="B105" s="31">
-        <f>$D$43*(1+$B$54)^-A105*(1+$B$53)^A105</f>
-        <v>15676.811027479071</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B105" s="26">
+        <f t="shared" si="3"/>
+        <v>26009.179555392846</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="B106" s="31">
-        <f>$D$43*(1+$B$54)^-A106*(1+$B$53)^A106</f>
-        <v>15388.510649071284</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B106" s="26">
+        <f t="shared" si="3"/>
+        <v>25530.864399666836</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>51</v>
       </c>
-      <c r="B107" s="31">
-        <f>$D$43*(1+$B$54)^-A107*(1+$B$53)^A107</f>
-        <v>15105.512184939584</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B107" s="26">
+        <f t="shared" si="3"/>
+        <v>25061.345576316871</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
-      <c r="B108" s="31">
-        <f>$D$43*(1+$B$54)^-A108*(1+$B$53)^A108</f>
-        <v>14827.718131587282</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B108" s="26">
+        <f t="shared" si="3"/>
+        <v>24600.461318645095</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>53</v>
       </c>
-      <c r="B109" s="31">
-        <f>$D$43*(1+$B$54)^-A109*(1+$B$53)^A109</f>
-        <v>14555.032778630777</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B109" s="26">
+        <f t="shared" si="3"/>
+        <v>24148.052834882699</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
-      <c r="B110" s="31">
-        <f>$D$43*(1+$B$54)^-A110*(1+$B$53)^A110</f>
-        <v>14287.362175823766</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B110" s="26">
+        <f t="shared" si="3"/>
+        <v>23703.964253480226</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>55</v>
       </c>
-      <c r="B111" s="31">
-        <f>$D$43*(1+$B$54)^-A111*(1+$B$53)^A111</f>
-        <v>14024.614100687882</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B111" s="26">
+        <f t="shared" si="3"/>
+        <v>23268.042569404028</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>56</v>
       </c>
-      <c r="B112" s="31">
-        <f>$D$43*(1+$B$54)^-A112*(1+$B$53)^A112</f>
-        <v>13766.698026738652</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B112" s="26">
+        <f t="shared" si="3"/>
+        <v>22840.13759142036</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>57</v>
       </c>
-      <c r="B113" s="31">
-        <f>$D$43*(1+$B$54)^-A113*(1+$B$53)^A113</f>
-        <v>13513.525092295704</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B113" s="26">
+        <f t="shared" si="3"/>
+        <v>22420.101890348877</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114">
         <f>A113+1</f>
         <v>58</v>
       </c>
-      <c r="B114" s="31">
-        <f>$D$43*(1+$B$54)^-A114*(1+$B$53)^A114</f>
-        <v>13265.008069866657</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B114" s="26">
+        <f t="shared" si="3"/>
+        <v>22007.790748267831</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>59</v>
       </c>
-      <c r="B115" s="31">
-        <f>$D$43*(1+$B$54)^-A115*(1+$B$53)^A115</f>
-        <v>13021.061336093986</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B115" s="26">
+        <f t="shared" si="3"/>
+        <v>21603.062108653339</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="B116" s="31">
-        <f>$D$43*(1+$B$54)^-A116*(1+$B$53)^A116</f>
-        <v>12781.600842254606</v>
+      <c r="B116" s="26">
+        <f t="shared" si="3"/>
+        <v>21205.776527435679</v>
       </c>
     </row>
   </sheetData>
@@ -2711,47 +2629,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60C3FA1-C501-488F-99EF-B28CB9021ECA}">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="55" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
-    <col min="4" max="4" width="19.5" customWidth="1"/>
-    <col min="6" max="6" width="29.5" customWidth="1"/>
-    <col min="7" max="7" width="12.5" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="19.1796875" customWidth="1"/>
+    <col min="4" max="4" width="19.453125" customWidth="1"/>
+    <col min="6" max="6" width="29.453125" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" customWidth="1"/>
+    <col min="8" max="8" width="15.6328125" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" customWidth="1"/>
-    <col min="15" max="15" width="12.5" customWidth="1"/>
-    <col min="17" max="17" width="12.83203125" customWidth="1"/>
+    <col min="10" max="10" width="14.453125" customWidth="1"/>
+    <col min="11" max="11" width="12.81640625" customWidth="1"/>
+    <col min="12" max="12" width="10.6328125" customWidth="1"/>
+    <col min="13" max="13" width="11.6328125" customWidth="1"/>
+    <col min="15" max="15" width="12.453125" customWidth="1"/>
+    <col min="17" max="17" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="2">
         <f>10*D11</f>
         <v>21040</v>
       </c>
@@ -2759,12 +2677,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="2">
         <f xml:space="preserve"> 0.05*C3</f>
         <v>1052</v>
       </c>
@@ -2775,12 +2693,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <f>SUM(C3:C4)</f>
         <v>22092</v>
       </c>
@@ -2791,7 +2709,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="F6" t="s">
         <v>58</v>
@@ -2800,12 +2718,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="45">
+      <c r="C7" s="40">
         <f>C5*52</f>
         <v>1148784</v>
       </c>
@@ -2816,7 +2734,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="F8" t="s">
         <v>61</v>
@@ -2824,8 +2742,11 @@
       <c r="G8">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H8" s="33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="F9" t="s">
         <v>62</v>
@@ -2833,31 +2754,28 @@
       <c r="G9">
         <v>27</v>
       </c>
-      <c r="H9" s="38" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="G10" s="6"/>
+      <c r="D10" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="5"/>
+      <c r="J10" s="4"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="5"/>
-    </row>
-    <row r="11" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="M10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="36" t="s">
         <v>4</v>
       </c>
       <c r="C11">
@@ -2869,18 +2787,18 @@
       <c r="F11" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="1">
         <v>25</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="5"/>
+      <c r="J11" s="4"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="5"/>
-    </row>
-    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="B12" s="41" t="s">
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B12" s="36" t="s">
         <v>49</v>
       </c>
       <c r="C12">
@@ -2892,18 +2810,18 @@
       <c r="F12" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="1">
         <v>20</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="5"/>
+      <c r="J12" s="4"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="5"/>
-    </row>
-    <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="B13" s="41" t="s">
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B13" s="36" t="s">
         <v>7</v>
       </c>
       <c r="C13">
@@ -2912,16 +2830,16 @@
       <c r="D13">
         <v>3514</v>
       </c>
-      <c r="G13" s="6"/>
+      <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="5"/>
+      <c r="J13" s="4"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="5"/>
-    </row>
-    <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="B14" s="41" t="s">
+      <c r="M13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B14" s="36" t="s">
         <v>6</v>
       </c>
       <c r="C14">
@@ -2931,20 +2849,20 @@
         <v>265</v>
       </c>
       <c r="F14" t="s">
-        <v>80</v>
-      </c>
-      <c r="G14" s="6">
+        <v>78</v>
+      </c>
+      <c r="G14" s="1">
         <v>6.1500000000000001E-3</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="5"/>
+      <c r="J14" s="4"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="5"/>
-    </row>
-    <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="B15" s="41" t="s">
+      <c r="M14" s="4"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B15" s="36" t="s">
         <v>53</v>
       </c>
       <c r="C15">
@@ -2955,34 +2873,34 @@
         <f>SUM(D11:D14)</f>
         <v>8972</v>
       </c>
-      <c r="G15" s="6"/>
+      <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="5"/>
+      <c r="J15" s="4"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="5"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
-      <c r="G16" s="6"/>
+      <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="5"/>
+      <c r="J16" s="4"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="5"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="G17" s="6"/>
+      <c r="M16" s="4"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="5"/>
+      <c r="J17" s="4"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="5"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M17" s="4"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -2992,47 +2910,45 @@
       <c r="J18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="G19" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="J19" s="38" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="G20" s="25"/>
-      <c r="H20" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="J19" s="33"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="G20" s="21"/>
+      <c r="H20" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20" t="s">
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q20" s="26"/>
-    </row>
-    <row r="21" spans="1:17" ht="80" x14ac:dyDescent="0.2">
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q20" s="22"/>
+    </row>
+    <row r="21" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="F21" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J21" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="J21" s="4" t="s">
         <v>73</v>
       </c>
       <c r="K21" s="1" t="s">
@@ -3047,55 +2963,53 @@
       <c r="N21" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="O21" s="5" t="s">
+      <c r="O21" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B22" s="1"/>
       <c r="F22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="7">
         <v>23.3</v>
       </c>
-      <c r="H22" s="30">
-        <f>(C11*G8)/60</f>
-        <v>967.86666666666667</v>
-      </c>
-      <c r="I22" s="43">
-        <f>D11*G8/60</f>
-        <v>596.13333333333333</v>
-      </c>
-      <c r="J22" s="44">
-        <f>(H22-I22)*G22</f>
-        <v>8661.3866666666672</v>
+      <c r="H22" s="15">
+        <v>0</v>
+      </c>
+      <c r="I22" s="38">
+        <v>0</v>
+      </c>
+      <c r="J22" s="39">
+        <f>H22+I22</f>
+        <v>0</v>
       </c>
       <c r="K22">
         <f>C11*G4-D11*G4</f>
         <v>15744</v>
       </c>
-      <c r="L22" s="10">
+      <c r="L22" s="7">
         <v>192</v>
       </c>
       <c r="M22">
         <f>L22/1000000</f>
         <v>1.92E-4</v>
       </c>
-      <c r="N22" s="10">
+      <c r="N22" s="7">
         <v>90</v>
       </c>
       <c r="O22" s="3">
         <f>K22*M22*N22</f>
         <v>272.05632000000003</v>
       </c>
-      <c r="P22" s="10">
+      <c r="P22" s="7">
         <f>(0.012+0.031)/2</f>
         <v>2.1499999999999998E-2</v>
       </c>
@@ -3104,7 +3018,7 @@
         <v>338.49599999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>0</v>
       </c>
@@ -3118,71 +3032,70 @@
       <c r="F23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G23" s="10">
+      <c r="G23" s="7">
         <v>14.4</v>
       </c>
       <c r="H23">
-        <f>(C12*G9)/60</f>
-        <v>1233.9000000000001</v>
-      </c>
-      <c r="I23" s="43">
-        <f>D12*G9/60</f>
-        <v>1390.05</v>
-      </c>
-      <c r="J23" s="44">
-        <f>(H23-I23)*G23</f>
-        <v>-2248.5599999999981</v>
+        <v>0</v>
+      </c>
+      <c r="I23" s="38">
+        <f>0.5*(D12-C12)*G9*(G22-G23)/60</f>
+        <v>694.86750000000006</v>
+      </c>
+      <c r="J23" s="39">
+        <f>H23+I23</f>
+        <v>694.86750000000006</v>
       </c>
       <c r="K23">
-        <f>D12*G5-C12*G5</f>
-        <v>4164</v>
-      </c>
-      <c r="L23" s="10">
+        <f>C12*G5-D12*G5</f>
+        <v>-4164</v>
+      </c>
+      <c r="L23" s="7">
         <v>35</v>
       </c>
       <c r="M23">
         <f t="shared" ref="M23:M25" si="0">L23/1000000</f>
         <v>3.4999999999999997E-5</v>
       </c>
-      <c r="N23" s="10">
+      <c r="N23" s="7">
         <v>90</v>
       </c>
       <c r="O23" s="3">
         <f>K23*M23*N23</f>
-        <v>13.116599999999998</v>
+        <v>-13.116599999999998</v>
       </c>
       <c r="P23">
         <v>0</v>
       </c>
-      <c r="Q23" s="22"/>
-    </row>
-    <row r="24" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="Q23" s="19"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="2">
         <f>SUM(J22:J25)</f>
-        <v>6412.8266666666696</v>
+        <v>694.86750000000006</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="21"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
       <c r="K24">
         <f>D13*G6-C13*G6</f>
         <v>790</v>
       </c>
-      <c r="L24" s="10">
+      <c r="L24" s="7">
         <v>0</v>
       </c>
       <c r="M24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N24" s="10">
+      <c r="N24" s="7">
         <v>90</v>
       </c>
       <c r="O24" s="3">
@@ -3192,35 +3105,35 @@
       <c r="P24">
         <v>0</v>
       </c>
-      <c r="Q24" s="22"/>
-    </row>
-    <row r="25" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="Q24" s="19"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B25" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="2">
         <f>SUM(O22:O25)</f>
-        <v>285.17292000000003</v>
+        <v>258.93972000000002</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="21"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
       <c r="K25">
         <f>D14*G7-C14*G7</f>
         <v>150</v>
       </c>
-      <c r="L25" s="10">
+      <c r="L25" s="7">
         <v>0</v>
       </c>
       <c r="M25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N25" s="10">
+      <c r="N25" s="7">
         <v>90</v>
       </c>
       <c r="O25" s="3">
@@ -3230,73 +3143,73 @@
       <c r="P25">
         <v>0</v>
       </c>
-      <c r="Q25" s="22"/>
-    </row>
-    <row r="26" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="Q25" s="19"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B26" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C26" s="2">
         <f>SUM(Q22:Q25)</f>
         <v>338.49599999999998</v>
       </c>
       <c r="F26" s="1"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="L26" s="10"/>
-      <c r="N26" s="10"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="L26" s="7"/>
+      <c r="N26" s="7"/>
       <c r="O26" s="3"/>
-      <c r="Q26" s="22"/>
-    </row>
-    <row r="27" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="B27" s="5" t="s">
+      <c r="Q26" s="19"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B27" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="5">
         <f>SUM(C23:C26)</f>
-        <v>28076.495586666668</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B28" s="5"/>
-      <c r="C28" s="7"/>
-    </row>
-    <row r="29" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>22332.303219999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="45">
+      <c r="C29" s="40">
         <f>C27*52</f>
-        <v>1459977.7705066667</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+        <v>1161279.7674399999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A31" s="48" t="s">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A31" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="49">
+      <c r="B31" s="44">
         <f>C29/C7</f>
-        <v>1.2708897151306657</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+        <v>1.0108773863842113</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected (hope so) cost allocation for the car tax project
</commit_message>
<xml_diff>
--- a/CBA.xlsx
+++ b/CBA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a630b34756993743/Desktop/ETHZ/Transport Planning Methods/TransportPlanning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{7917CEA6-7AB6-7840-849C-A049323EA15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{639C19C6-FF23-405D-9C4D-9B1F9CF64131}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{7917CEA6-7AB6-7840-849C-A049323EA15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F11DC383-6E96-4771-AA90-3C54739522D1}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CB19214C-161C-4FCD-BB74-FBBD26C9B7EC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{CB19214C-161C-4FCD-BB74-FBBD26C9B7EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Project 2" sheetId="1" r:id="rId1"/>
@@ -305,7 +305,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="101">
   <si>
     <t>Weekly benefits</t>
   </si>
@@ -657,6 +657,9 @@
   </si>
   <si>
     <t>Current adult population of Canton Zurich</t>
+  </si>
+  <si>
+    <t>Cost of tax to drivers (counted as a negative benefit)</t>
   </si>
 </sst>
 </file>
@@ -852,7 +855,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -927,7 +930,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -948,6 +950,10 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -1250,8 +1256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D083A40F-175A-4EEC-B4D7-09BE1D9F546C}">
   <dimension ref="A1:R116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="74" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView topLeftCell="A28" zoomScale="74" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1681,7 +1687,7 @@
       <c r="G30" t="s">
         <v>99</v>
       </c>
-      <c r="H30" s="46">
+      <c r="H30" s="7">
         <v>1240000</v>
       </c>
     </row>
@@ -2653,10 +2659,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60C3FA1-C501-488F-99EF-B28CB9021ECA}">
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView zoomScale="55" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="55" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2688,16 +2694,16 @@
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="C3" s="2">
-        <f>10*D11</f>
-        <v>21040</v>
+        <f>10*D11*G15*8/1254</f>
+        <v>166440829.34609249</v>
       </c>
       <c r="F3" t="s">
         <v>55</v>
@@ -2710,7 +2716,7 @@
       </c>
       <c r="C4" s="2">
         <f xml:space="preserve"> 0.05*C3</f>
-        <v>1052</v>
+        <v>8322041.4673046246</v>
       </c>
       <c r="F4" t="s">
         <v>56</v>
@@ -2725,8 +2731,8 @@
         <v>12</v>
       </c>
       <c r="C5" s="5">
-        <f>SUM(C3:C4)</f>
-        <v>22092</v>
+        <f>C4</f>
+        <v>8322041.4673046246</v>
       </c>
       <c r="F5" t="s">
         <v>57</v>
@@ -2751,7 +2757,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="40">
         <f>C5*52</f>
-        <v>1148784</v>
+        <v>432746156.29984045</v>
       </c>
       <c r="F7" t="s">
         <v>59</v>
@@ -2899,7 +2905,12 @@
         <f>SUM(D11:D14)</f>
         <v>8972</v>
       </c>
-      <c r="G15" s="1"/>
+      <c r="F15" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" s="7">
+        <v>1240000</v>
+      </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="4"/>
@@ -3049,11 +3060,11 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C23" s="2">
-        <f>10*D11</f>
-        <v>21040</v>
+        <f>-10*D11*G15*8/1254</f>
+        <v>-166440829.34609249</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>5</v>
@@ -3097,11 +3108,11 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C24" s="2">
-        <f>SUM(J22:J25)</f>
-        <v>694.86750000000006</v>
+        <f>10*D11*G15*8/1254</f>
+        <v>166440829.34609249</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>7</v>
@@ -3135,11 +3146,11 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B25" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C25" s="2">
-        <f>SUM(O22:O25)</f>
-        <v>258.93972000000002</v>
+        <f>SUM(J22:J25)*G15*8/1254</f>
+        <v>5496878.468899522</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>6</v>
@@ -3173,11 +3184,11 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B26" s="1" t="s">
-        <v>91</v>
+        <v>9</v>
       </c>
       <c r="C26" s="2">
-        <f>SUM(Q22:Q25)</f>
-        <v>338.49599999999998</v>
+        <f>SUM(O22:O25)*G15*8/1254</f>
+        <v>2048390.7674641148</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="18"/>
@@ -3190,53 +3201,62 @@
       <c r="Q26" s="19"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="2">
+        <f>SUM(Q22:Q25)*G15*8/1254</f>
+        <v>2677735.5023923446</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B28" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="5">
-        <f>SUM(C23:C26)</f>
-        <v>22332.303219999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B28" s="4"/>
-      <c r="C28" s="5"/>
+      <c r="C28" s="5">
+        <f>SUM(C24:C27)</f>
+        <v>176663834.08484846</v>
+      </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>94</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B30" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="40">
-        <f>C27*52</f>
-        <v>1161279.7674399999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B30" s="1"/>
+      <c r="C30" s="40">
+        <f>C28*52</f>
+        <v>9186519372.4121208</v>
+      </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="44">
-        <f>C29/C7</f>
-        <v>1.0108773863842113</v>
-      </c>
-      <c r="C31" s="8" t="s">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B32" s="44">
+        <f>C30/C7</f>
+        <v>21.228425114068443</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B32" s="1"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="1"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>